<commit_message>
2016-05-12掠夺(防守-杭州-雨字-白龙瀑分舵) PIC OCR Convert & Summary Update
</commit_message>
<xml_diff>
--- a/5.9-5.15.xlsx
+++ b/5.9-5.15.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="215">
   <si>
     <t>ID</t>
   </si>
@@ -662,6 +662,21 @@
   </si>
   <si>
     <t>再见是否红着脸</t>
+  </si>
+  <si>
+    <t>骄傲的龙王丶</t>
+  </si>
+  <si>
+    <t>池小晩</t>
+  </si>
+  <si>
+    <t>大叔别跑啊</t>
+  </si>
+  <si>
+    <t>梦太晩</t>
+  </si>
+  <si>
+    <t>璐小虫</t>
   </si>
 </sst>
 </file>
@@ -1024,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,6 +1050,7 @@
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="3"/>
     <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
     <col min="17" max="17" width="9.140625" style="3"/>
     <col min="18" max="18" width="17.42578125" customWidth="1"/>
   </cols>
@@ -1132,6 +1148,12 @@
       <c r="J3" t="s">
         <v>95</v>
       </c>
+      <c r="M3" s="3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>32</v>
+      </c>
       <c r="Q3" s="3">
         <v>1</v>
       </c>
@@ -1158,6 +1180,12 @@
       <c r="J4" t="s">
         <v>57</v>
       </c>
+      <c r="M4" s="3">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>36</v>
+      </c>
       <c r="Q4" s="3">
         <v>2</v>
       </c>
@@ -1184,6 +1212,12 @@
       <c r="J5" t="s">
         <v>29</v>
       </c>
+      <c r="M5" s="3">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>40</v>
+      </c>
       <c r="Q5" s="3">
         <v>3</v>
       </c>
@@ -1210,6 +1244,12 @@
       <c r="J6" t="s">
         <v>36</v>
       </c>
+      <c r="M6" s="3">
+        <v>4</v>
+      </c>
+      <c r="N6" t="s">
+        <v>204</v>
+      </c>
       <c r="Q6" s="3">
         <v>4</v>
       </c>
@@ -1236,6 +1276,12 @@
       <c r="J7" t="s">
         <v>71</v>
       </c>
+      <c r="M7" s="3">
+        <v>5</v>
+      </c>
+      <c r="N7" t="s">
+        <v>98</v>
+      </c>
       <c r="Q7" s="3">
         <v>5</v>
       </c>
@@ -1262,6 +1308,12 @@
       <c r="J8" t="s">
         <v>56</v>
       </c>
+      <c r="M8" s="3">
+        <v>6</v>
+      </c>
+      <c r="N8" t="s">
+        <v>194</v>
+      </c>
       <c r="Q8" s="3">
         <v>6</v>
       </c>
@@ -1288,6 +1340,12 @@
       <c r="J9" t="s">
         <v>84</v>
       </c>
+      <c r="M9" s="3">
+        <v>7</v>
+      </c>
+      <c r="N9" t="s">
+        <v>52</v>
+      </c>
       <c r="Q9" s="3">
         <v>7</v>
       </c>
@@ -1314,6 +1372,12 @@
       <c r="J10" t="s">
         <v>151</v>
       </c>
+      <c r="M10" s="3">
+        <v>8</v>
+      </c>
+      <c r="N10" t="s">
+        <v>142</v>
+      </c>
       <c r="Q10" s="3">
         <v>8</v>
       </c>
@@ -1340,6 +1404,12 @@
       <c r="J11" t="s">
         <v>89</v>
       </c>
+      <c r="M11" s="3">
+        <v>9</v>
+      </c>
+      <c r="N11" t="s">
+        <v>104</v>
+      </c>
       <c r="Q11" s="3">
         <v>9</v>
       </c>
@@ -1366,6 +1436,12 @@
       <c r="J12" t="s">
         <v>88</v>
       </c>
+      <c r="M12" s="3">
+        <v>10</v>
+      </c>
+      <c r="N12" t="s">
+        <v>97</v>
+      </c>
       <c r="Q12" s="3">
         <v>10</v>
       </c>
@@ -1392,6 +1468,12 @@
       <c r="J13" t="s">
         <v>47</v>
       </c>
+      <c r="M13" s="3">
+        <v>11</v>
+      </c>
+      <c r="N13" t="s">
+        <v>56</v>
+      </c>
       <c r="Q13" s="3">
         <v>11</v>
       </c>
@@ -1418,6 +1500,12 @@
       <c r="J14" t="s">
         <v>152</v>
       </c>
+      <c r="M14" s="3">
+        <v>12</v>
+      </c>
+      <c r="N14" t="s">
+        <v>60</v>
+      </c>
       <c r="Q14" s="3">
         <v>12</v>
       </c>
@@ -1444,6 +1532,12 @@
       <c r="J15" t="s">
         <v>109</v>
       </c>
+      <c r="M15" s="3">
+        <v>13</v>
+      </c>
+      <c r="N15" t="s">
+        <v>24</v>
+      </c>
       <c r="Q15" s="3">
         <v>13</v>
       </c>
@@ -1470,6 +1564,12 @@
       <c r="J16" t="s">
         <v>74</v>
       </c>
+      <c r="M16" s="3">
+        <v>14</v>
+      </c>
+      <c r="N16" t="s">
+        <v>184</v>
+      </c>
       <c r="Q16" s="3">
         <v>14</v>
       </c>
@@ -1496,6 +1596,12 @@
       <c r="J17" t="s">
         <v>142</v>
       </c>
+      <c r="M17" s="3">
+        <v>15</v>
+      </c>
+      <c r="N17" t="s">
+        <v>149</v>
+      </c>
       <c r="Q17" s="3">
         <v>15</v>
       </c>
@@ -1522,6 +1628,12 @@
       <c r="J18" t="s">
         <v>150</v>
       </c>
+      <c r="M18" s="3">
+        <v>16</v>
+      </c>
+      <c r="N18" t="s">
+        <v>64</v>
+      </c>
       <c r="Q18" s="3">
         <v>16</v>
       </c>
@@ -1548,6 +1660,12 @@
       <c r="J19" t="s">
         <v>40</v>
       </c>
+      <c r="M19" s="3">
+        <v>17</v>
+      </c>
+      <c r="N19" t="s">
+        <v>185</v>
+      </c>
       <c r="Q19" s="3">
         <v>17</v>
       </c>
@@ -1574,6 +1692,12 @@
       <c r="J20" t="s">
         <v>153</v>
       </c>
+      <c r="M20" s="3">
+        <v>18</v>
+      </c>
+      <c r="N20" t="s">
+        <v>48</v>
+      </c>
       <c r="Q20" s="3">
         <v>18</v>
       </c>
@@ -1600,6 +1724,12 @@
       <c r="J21" t="s">
         <v>112</v>
       </c>
+      <c r="M21" s="3">
+        <v>19</v>
+      </c>
+      <c r="N21" t="s">
+        <v>72</v>
+      </c>
       <c r="Q21" s="3">
         <v>19</v>
       </c>
@@ -1626,6 +1756,12 @@
       <c r="J22" t="s">
         <v>38</v>
       </c>
+      <c r="M22" s="3">
+        <v>20</v>
+      </c>
+      <c r="N22" t="s">
+        <v>76</v>
+      </c>
       <c r="Q22" s="3">
         <v>20</v>
       </c>
@@ -1652,6 +1788,12 @@
       <c r="J23" t="s">
         <v>85</v>
       </c>
+      <c r="M23" s="3">
+        <v>21</v>
+      </c>
+      <c r="N23" t="s">
+        <v>210</v>
+      </c>
       <c r="Q23" s="3">
         <v>21</v>
       </c>
@@ -1678,6 +1820,12 @@
       <c r="J24" t="s">
         <v>53</v>
       </c>
+      <c r="M24" s="3">
+        <v>22</v>
+      </c>
+      <c r="N24" t="s">
+        <v>33</v>
+      </c>
       <c r="Q24" s="3">
         <v>22</v>
       </c>
@@ -1704,6 +1852,12 @@
       <c r="J25" t="s">
         <v>91</v>
       </c>
+      <c r="M25" s="3">
+        <v>23</v>
+      </c>
+      <c r="N25" t="s">
+        <v>99</v>
+      </c>
       <c r="Q25" s="3">
         <v>23</v>
       </c>
@@ -1730,6 +1884,12 @@
       <c r="J26" t="s">
         <v>100</v>
       </c>
+      <c r="M26" s="3">
+        <v>24</v>
+      </c>
+      <c r="N26" t="s">
+        <v>144</v>
+      </c>
       <c r="Q26" s="3">
         <v>24</v>
       </c>
@@ -1756,6 +1916,12 @@
       <c r="J27" t="s">
         <v>149</v>
       </c>
+      <c r="M27" s="3">
+        <v>25</v>
+      </c>
+      <c r="N27" t="s">
+        <v>101</v>
+      </c>
       <c r="Q27" s="3">
         <v>25</v>
       </c>
@@ -1782,6 +1948,12 @@
       <c r="J28" t="s">
         <v>45</v>
       </c>
+      <c r="M28" s="3">
+        <v>26</v>
+      </c>
+      <c r="N28" t="s">
+        <v>45</v>
+      </c>
       <c r="Q28" s="3">
         <v>26</v>
       </c>
@@ -1808,6 +1980,12 @@
       <c r="J29" t="s">
         <v>113</v>
       </c>
+      <c r="M29" s="3">
+        <v>27</v>
+      </c>
+      <c r="N29" t="s">
+        <v>49</v>
+      </c>
       <c r="Q29" s="3">
         <v>27</v>
       </c>
@@ -1834,6 +2012,12 @@
       <c r="J30" t="s">
         <v>97</v>
       </c>
+      <c r="M30" s="3">
+        <v>28</v>
+      </c>
+      <c r="N30" t="s">
+        <v>25</v>
+      </c>
       <c r="Q30" s="3">
         <v>28</v>
       </c>
@@ -1860,6 +2044,12 @@
       <c r="J31" t="s">
         <v>114</v>
       </c>
+      <c r="M31" s="3">
+        <v>29</v>
+      </c>
+      <c r="N31" t="s">
+        <v>57</v>
+      </c>
       <c r="Q31" s="3">
         <v>29</v>
       </c>
@@ -1886,6 +2076,12 @@
       <c r="J32" t="s">
         <v>63</v>
       </c>
+      <c r="M32" s="3">
+        <v>30</v>
+      </c>
+      <c r="N32" t="s">
+        <v>73</v>
+      </c>
       <c r="Q32" s="3">
         <v>30</v>
       </c>
@@ -1912,6 +2108,12 @@
       <c r="J33" t="s">
         <v>154</v>
       </c>
+      <c r="M33" s="3">
+        <v>31</v>
+      </c>
+      <c r="N33" t="s">
+        <v>107</v>
+      </c>
       <c r="Q33" s="3">
         <v>31</v>
       </c>
@@ -1938,6 +2140,12 @@
       <c r="J34" t="s">
         <v>155</v>
       </c>
+      <c r="M34" s="3">
+        <v>32</v>
+      </c>
+      <c r="N34" t="s">
+        <v>53</v>
+      </c>
       <c r="Q34" s="3">
         <v>32</v>
       </c>
@@ -1964,6 +2172,12 @@
       <c r="J35" t="s">
         <v>135</v>
       </c>
+      <c r="M35" s="3">
+        <v>33</v>
+      </c>
+      <c r="N35" t="s">
+        <v>192</v>
+      </c>
       <c r="Q35" s="3">
         <v>33</v>
       </c>
@@ -1990,6 +2204,12 @@
       <c r="J36" t="s">
         <v>72</v>
       </c>
+      <c r="M36" s="3">
+        <v>34</v>
+      </c>
+      <c r="N36" t="s">
+        <v>171</v>
+      </c>
       <c r="Q36" s="3">
         <v>34</v>
       </c>
@@ -2016,6 +2236,12 @@
       <c r="J37" t="s">
         <v>61</v>
       </c>
+      <c r="M37" s="3">
+        <v>35</v>
+      </c>
+      <c r="N37" t="s">
+        <v>193</v>
+      </c>
       <c r="Q37" s="3">
         <v>35</v>
       </c>
@@ -2042,6 +2268,12 @@
       <c r="J38" t="s">
         <v>156</v>
       </c>
+      <c r="M38" s="3">
+        <v>36</v>
+      </c>
+      <c r="N38" t="s">
+        <v>69</v>
+      </c>
       <c r="Q38" s="3">
         <v>36</v>
       </c>
@@ -2068,6 +2300,12 @@
       <c r="J39" t="s">
         <v>157</v>
       </c>
+      <c r="M39" s="3">
+        <v>37</v>
+      </c>
+      <c r="N39" t="s">
+        <v>134</v>
+      </c>
       <c r="Q39" s="3">
         <v>37</v>
       </c>
@@ -2094,6 +2332,12 @@
       <c r="J40" t="s">
         <v>79</v>
       </c>
+      <c r="M40" s="3">
+        <v>38</v>
+      </c>
+      <c r="N40" t="s">
+        <v>146</v>
+      </c>
       <c r="Q40" s="3">
         <v>38</v>
       </c>
@@ -2120,6 +2364,12 @@
       <c r="J41" t="s">
         <v>120</v>
       </c>
+      <c r="M41" s="3">
+        <v>39</v>
+      </c>
+      <c r="N41" t="s">
+        <v>211</v>
+      </c>
       <c r="Q41" s="3">
         <v>39</v>
       </c>
@@ -2146,6 +2396,12 @@
       <c r="J42" t="s">
         <v>87</v>
       </c>
+      <c r="M42" s="3">
+        <v>40</v>
+      </c>
+      <c r="N42" t="s">
+        <v>141</v>
+      </c>
       <c r="Q42" s="3">
         <v>40</v>
       </c>
@@ -2172,6 +2428,12 @@
       <c r="J43" t="s">
         <v>145</v>
       </c>
+      <c r="M43" s="3">
+        <v>41</v>
+      </c>
+      <c r="N43" t="s">
+        <v>77</v>
+      </c>
       <c r="Q43" s="3">
         <v>41</v>
       </c>
@@ -2198,6 +2460,12 @@
       <c r="J44" t="s">
         <v>60</v>
       </c>
+      <c r="M44" s="3">
+        <v>42</v>
+      </c>
+      <c r="N44" t="s">
+        <v>81</v>
+      </c>
       <c r="Q44" s="3">
         <v>42</v>
       </c>
@@ -2224,6 +2492,12 @@
       <c r="J45" t="s">
         <v>62</v>
       </c>
+      <c r="M45" s="3">
+        <v>43</v>
+      </c>
+      <c r="N45" t="s">
+        <v>88</v>
+      </c>
       <c r="Q45" s="3">
         <v>43</v>
       </c>
@@ -2250,6 +2524,12 @@
       <c r="J46" t="s">
         <v>98</v>
       </c>
+      <c r="M46" s="3">
+        <v>44</v>
+      </c>
+      <c r="N46" t="s">
+        <v>207</v>
+      </c>
       <c r="Q46" s="3">
         <v>44</v>
       </c>
@@ -2276,6 +2556,12 @@
       <c r="J47" t="s">
         <v>158</v>
       </c>
+      <c r="M47" s="3">
+        <v>45</v>
+      </c>
+      <c r="N47" t="s">
+        <v>172</v>
+      </c>
       <c r="Q47" s="3">
         <v>45</v>
       </c>
@@ -2302,6 +2588,12 @@
       <c r="J48" t="s">
         <v>73</v>
       </c>
+      <c r="M48" s="3">
+        <v>46</v>
+      </c>
+      <c r="N48" t="s">
+        <v>30</v>
+      </c>
       <c r="Q48" s="3">
         <v>46</v>
       </c>
@@ -2328,6 +2620,12 @@
       <c r="J49" t="s">
         <v>159</v>
       </c>
+      <c r="M49" s="3">
+        <v>47</v>
+      </c>
+      <c r="N49" t="s">
+        <v>38</v>
+      </c>
       <c r="Q49" s="3">
         <v>47</v>
       </c>
@@ -2354,6 +2652,12 @@
       <c r="J50" t="s">
         <v>103</v>
       </c>
+      <c r="M50" s="3">
+        <v>48</v>
+      </c>
+      <c r="N50" t="s">
+        <v>42</v>
+      </c>
       <c r="Q50" s="3">
         <v>48</v>
       </c>
@@ -2380,6 +2684,12 @@
       <c r="J51" t="s">
         <v>160</v>
       </c>
+      <c r="M51" s="3">
+        <v>49</v>
+      </c>
+      <c r="N51" t="s">
+        <v>174</v>
+      </c>
       <c r="Q51" s="3">
         <v>49</v>
       </c>
@@ -2406,6 +2716,12 @@
       <c r="J52" t="s">
         <v>161</v>
       </c>
+      <c r="M52" s="3">
+        <v>50</v>
+      </c>
+      <c r="N52" t="s">
+        <v>58</v>
+      </c>
       <c r="Q52" s="3">
         <v>50</v>
       </c>
@@ -2432,6 +2748,12 @@
       <c r="J53" t="s">
         <v>33</v>
       </c>
+      <c r="M53" s="3">
+        <v>51</v>
+      </c>
+      <c r="N53" t="s">
+        <v>212</v>
+      </c>
       <c r="Q53" s="3">
         <v>51</v>
       </c>
@@ -2458,6 +2780,12 @@
       <c r="J54" t="s">
         <v>67</v>
       </c>
+      <c r="M54" s="3">
+        <v>52</v>
+      </c>
+      <c r="N54" t="s">
+        <v>126</v>
+      </c>
       <c r="Q54" s="3">
         <v>52</v>
       </c>
@@ -2484,6 +2812,12 @@
       <c r="J55" t="s">
         <v>117</v>
       </c>
+      <c r="M55" s="3">
+        <v>53</v>
+      </c>
+      <c r="N55" t="s">
+        <v>131</v>
+      </c>
       <c r="Q55" s="3">
         <v>53</v>
       </c>
@@ -2510,6 +2844,12 @@
       <c r="J56" t="s">
         <v>108</v>
       </c>
+      <c r="M56" s="3">
+        <v>54</v>
+      </c>
+      <c r="N56" t="s">
+        <v>62</v>
+      </c>
       <c r="Q56" s="3">
         <v>54</v>
       </c>
@@ -2536,6 +2876,12 @@
       <c r="J57" t="s">
         <v>162</v>
       </c>
+      <c r="M57" s="3">
+        <v>55</v>
+      </c>
+      <c r="N57" t="s">
+        <v>125</v>
+      </c>
       <c r="Q57" s="3">
         <v>55</v>
       </c>
@@ -2562,6 +2908,12 @@
       <c r="J58" t="s">
         <v>163</v>
       </c>
+      <c r="M58" s="3">
+        <v>56</v>
+      </c>
+      <c r="N58" t="s">
+        <v>176</v>
+      </c>
       <c r="Q58" s="3">
         <v>56</v>
       </c>
@@ -2588,6 +2940,12 @@
       <c r="J59" t="s">
         <v>164</v>
       </c>
+      <c r="M59" s="3">
+        <v>57</v>
+      </c>
+      <c r="N59" t="s">
+        <v>113</v>
+      </c>
       <c r="Q59" s="3">
         <v>57</v>
       </c>
@@ -2614,6 +2972,12 @@
       <c r="J60" t="s">
         <v>125</v>
       </c>
+      <c r="M60" s="3">
+        <v>58</v>
+      </c>
+      <c r="N60" t="s">
+        <v>70</v>
+      </c>
       <c r="Q60" s="3">
         <v>58</v>
       </c>
@@ -2640,6 +3004,12 @@
       <c r="J61" t="s">
         <v>165</v>
       </c>
+      <c r="M61" s="3">
+        <v>59</v>
+      </c>
+      <c r="N61" t="s">
+        <v>182</v>
+      </c>
       <c r="Q61" s="3">
         <v>59</v>
       </c>
@@ -2666,6 +3036,12 @@
       <c r="J62" t="s">
         <v>141</v>
       </c>
+      <c r="M62" s="3">
+        <v>60</v>
+      </c>
+      <c r="N62" t="s">
+        <v>108</v>
+      </c>
       <c r="Q62" s="3">
         <v>60</v>
       </c>
@@ -2692,6 +3068,12 @@
       <c r="J63" t="s">
         <v>34</v>
       </c>
+      <c r="M63" s="3">
+        <v>61</v>
+      </c>
+      <c r="N63" t="s">
+        <v>138</v>
+      </c>
       <c r="Q63" s="3">
         <v>61</v>
       </c>
@@ -2718,6 +3100,12 @@
       <c r="J64" t="s">
         <v>41</v>
       </c>
+      <c r="M64" s="3">
+        <v>62</v>
+      </c>
+      <c r="N64" t="s">
+        <v>74</v>
+      </c>
       <c r="Q64" s="3">
         <v>62</v>
       </c>
@@ -2744,6 +3132,12 @@
       <c r="J65" t="s">
         <v>68</v>
       </c>
+      <c r="M65" s="3">
+        <v>63</v>
+      </c>
+      <c r="N65" t="s">
+        <v>78</v>
+      </c>
       <c r="Q65" s="3">
         <v>63</v>
       </c>
@@ -2770,6 +3164,12 @@
       <c r="J66" t="s">
         <v>30</v>
       </c>
+      <c r="M66" s="3">
+        <v>64</v>
+      </c>
+      <c r="N66" t="s">
+        <v>87</v>
+      </c>
       <c r="Q66" s="3">
         <v>64</v>
       </c>
@@ -2796,6 +3196,12 @@
       <c r="J67" t="s">
         <v>166</v>
       </c>
+      <c r="M67" s="3">
+        <v>65</v>
+      </c>
+      <c r="N67" t="s">
+        <v>89</v>
+      </c>
       <c r="Q67" s="3">
         <v>65</v>
       </c>
@@ -2822,6 +3228,12 @@
       <c r="J68" t="s">
         <v>167</v>
       </c>
+      <c r="M68" s="3">
+        <v>66</v>
+      </c>
+      <c r="N68" t="s">
+        <v>160</v>
+      </c>
       <c r="Q68" s="3">
         <v>66</v>
       </c>
@@ -2848,6 +3260,12 @@
       <c r="J69" t="s">
         <v>48</v>
       </c>
+      <c r="M69" s="3">
+        <v>67</v>
+      </c>
+      <c r="N69" t="s">
+        <v>143</v>
+      </c>
       <c r="Q69" s="3">
         <v>67</v>
       </c>
@@ -2874,6 +3292,12 @@
       <c r="J70" t="s">
         <v>92</v>
       </c>
+      <c r="M70" s="3">
+        <v>68</v>
+      </c>
+      <c r="N70" t="s">
+        <v>91</v>
+      </c>
       <c r="Q70" s="3">
         <v>68</v>
       </c>
@@ -2900,6 +3324,12 @@
       <c r="J71" t="s">
         <v>168</v>
       </c>
+      <c r="M71" s="3">
+        <v>69</v>
+      </c>
+      <c r="N71" t="s">
+        <v>92</v>
+      </c>
       <c r="Q71" s="3">
         <v>69</v>
       </c>
@@ -2926,6 +3356,12 @@
       <c r="J72" t="s">
         <v>128</v>
       </c>
+      <c r="M72" s="3">
+        <v>70</v>
+      </c>
+      <c r="N72" t="s">
+        <v>177</v>
+      </c>
       <c r="Q72" s="3">
         <v>70</v>
       </c>
@@ -2952,6 +3388,12 @@
       <c r="J73" t="s">
         <v>39</v>
       </c>
+      <c r="M73" s="3">
+        <v>71</v>
+      </c>
+      <c r="N73" t="s">
+        <v>203</v>
+      </c>
       <c r="Q73" s="3">
         <v>71</v>
       </c>
@@ -2978,6 +3420,12 @@
       <c r="J74" t="s">
         <v>169</v>
       </c>
+      <c r="M74" s="3">
+        <v>72</v>
+      </c>
+      <c r="N74" t="s">
+        <v>186</v>
+      </c>
       <c r="Q74" s="3">
         <v>72</v>
       </c>
@@ -3004,6 +3452,12 @@
       <c r="J75" t="s">
         <v>170</v>
       </c>
+      <c r="M75" s="3">
+        <v>73</v>
+      </c>
+      <c r="N75" t="s">
+        <v>140</v>
+      </c>
       <c r="Q75" s="3">
         <v>73</v>
       </c>
@@ -3030,6 +3484,12 @@
       <c r="J76" t="s">
         <v>138</v>
       </c>
+      <c r="M76" s="3">
+        <v>74</v>
+      </c>
+      <c r="N76" t="s">
+        <v>100</v>
+      </c>
       <c r="Q76" s="3">
         <v>74</v>
       </c>
@@ -3056,6 +3516,12 @@
       <c r="J77" t="s">
         <v>171</v>
       </c>
+      <c r="M77" s="3">
+        <v>75</v>
+      </c>
+      <c r="N77" t="s">
+        <v>145</v>
+      </c>
       <c r="Q77" s="3">
         <v>75</v>
       </c>
@@ -3082,6 +3548,12 @@
       <c r="J78" t="s">
         <v>172</v>
       </c>
+      <c r="M78" s="3">
+        <v>76</v>
+      </c>
+      <c r="N78" t="s">
+        <v>127</v>
+      </c>
       <c r="Q78" s="3">
         <v>76</v>
       </c>
@@ -3108,6 +3580,12 @@
       <c r="J79" t="s">
         <v>82</v>
       </c>
+      <c r="M79" s="3">
+        <v>77</v>
+      </c>
+      <c r="N79" t="s">
+        <v>180</v>
+      </c>
       <c r="Q79" s="3">
         <v>77</v>
       </c>
@@ -3134,6 +3612,12 @@
       <c r="J80" t="s">
         <v>32</v>
       </c>
+      <c r="M80" s="3">
+        <v>78</v>
+      </c>
+      <c r="N80" t="s">
+        <v>51</v>
+      </c>
       <c r="Q80" s="3">
         <v>78</v>
       </c>
@@ -3160,6 +3644,12 @@
       <c r="J81" t="s">
         <v>42</v>
       </c>
+      <c r="M81" s="3">
+        <v>79</v>
+      </c>
+      <c r="N81" t="s">
+        <v>55</v>
+      </c>
       <c r="Q81" s="3">
         <v>79</v>
       </c>
@@ -3186,6 +3676,12 @@
       <c r="J82" t="s">
         <v>144</v>
       </c>
+      <c r="M82" s="3">
+        <v>80</v>
+      </c>
+      <c r="N82" t="s">
+        <v>184</v>
+      </c>
       <c r="Q82" s="3">
         <v>80</v>
       </c>
@@ -3212,6 +3708,12 @@
       <c r="J83" t="s">
         <v>111</v>
       </c>
+      <c r="M83" s="3">
+        <v>81</v>
+      </c>
+      <c r="N83" t="s">
+        <v>63</v>
+      </c>
       <c r="Q83" s="3">
         <v>81</v>
       </c>
@@ -3238,6 +3740,12 @@
       <c r="J84" t="s">
         <v>131</v>
       </c>
+      <c r="M84" s="3">
+        <v>82</v>
+      </c>
+      <c r="N84" t="s">
+        <v>67</v>
+      </c>
       <c r="Q84" s="3">
         <v>82</v>
       </c>
@@ -3264,6 +3772,12 @@
       <c r="J85" t="s">
         <v>133</v>
       </c>
+      <c r="M85" s="3">
+        <v>83</v>
+      </c>
+      <c r="N85" t="s">
+        <v>213</v>
+      </c>
       <c r="Q85" s="3">
         <v>83</v>
       </c>
@@ -3290,6 +3804,12 @@
       <c r="J86" t="s">
         <v>132</v>
       </c>
+      <c r="M86" s="3">
+        <v>84</v>
+      </c>
+      <c r="N86" t="s">
+        <v>132</v>
+      </c>
       <c r="Q86" s="3">
         <v>84</v>
       </c>
@@ -3316,6 +3836,12 @@
       <c r="J87" t="s">
         <v>146</v>
       </c>
+      <c r="M87" s="3">
+        <v>85</v>
+      </c>
+      <c r="N87" t="s">
+        <v>71</v>
+      </c>
       <c r="Q87" s="3">
         <v>85</v>
       </c>
@@ -3342,6 +3868,12 @@
       <c r="J88" t="s">
         <v>83</v>
       </c>
+      <c r="M88" s="3">
+        <v>86</v>
+      </c>
+      <c r="N88" t="s">
+        <v>197</v>
+      </c>
       <c r="Q88" s="3">
         <v>86</v>
       </c>
@@ -3368,6 +3900,12 @@
       <c r="J89" t="s">
         <v>173</v>
       </c>
+      <c r="M89" s="3">
+        <v>87</v>
+      </c>
+      <c r="N89" t="s">
+        <v>119</v>
+      </c>
       <c r="Q89" s="3">
         <v>87</v>
       </c>
@@ -3394,6 +3932,12 @@
       <c r="J90" t="s">
         <v>115</v>
       </c>
+      <c r="M90" s="3">
+        <v>88</v>
+      </c>
+      <c r="N90" t="s">
+        <v>96</v>
+      </c>
       <c r="Q90" s="3">
         <v>88</v>
       </c>
@@ -3420,6 +3964,12 @@
       <c r="J91" t="s">
         <v>174</v>
       </c>
+      <c r="M91" s="3">
+        <v>89</v>
+      </c>
+      <c r="N91" t="s">
+        <v>214</v>
+      </c>
       <c r="Q91" s="3">
         <v>89</v>
       </c>
@@ -3446,6 +3996,12 @@
       <c r="J92" t="s">
         <v>25</v>
       </c>
+      <c r="M92" s="3">
+        <v>90</v>
+      </c>
+      <c r="N92" t="s">
+        <v>158</v>
+      </c>
       <c r="Q92" s="3">
         <v>90</v>
       </c>
@@ -3472,6 +4028,12 @@
       <c r="J93" t="s">
         <v>175</v>
       </c>
+      <c r="M93" s="3">
+        <v>91</v>
+      </c>
+      <c r="N93" t="s">
+        <v>79</v>
+      </c>
       <c r="Q93" s="3">
         <v>91</v>
       </c>
@@ -3498,6 +4060,12 @@
       <c r="J94" t="s">
         <v>24</v>
       </c>
+      <c r="M94" s="3">
+        <v>92</v>
+      </c>
+      <c r="N94" t="s">
+        <v>83</v>
+      </c>
       <c r="Q94" s="3">
         <v>92</v>
       </c>
@@ -3524,6 +4092,12 @@
       <c r="J95" t="s">
         <v>176</v>
       </c>
+      <c r="M95" s="3">
+        <v>93</v>
+      </c>
+      <c r="N95" t="s">
+        <v>112</v>
+      </c>
       <c r="Q95" s="3">
         <v>93</v>
       </c>
@@ -3550,6 +4124,12 @@
       <c r="J96" t="s">
         <v>177</v>
       </c>
+      <c r="M96" s="3">
+        <v>94</v>
+      </c>
+      <c r="N96" t="s">
+        <v>111</v>
+      </c>
       <c r="Q96" s="3">
         <v>94</v>
       </c>
@@ -3575,6 +4155,12 @@
       </c>
       <c r="J97" t="s">
         <v>35</v>
+      </c>
+      <c r="M97" s="3">
+        <v>95</v>
+      </c>
+      <c r="N97" t="s">
+        <v>126</v>
       </c>
       <c r="Q97" s="3">
         <v>95</v>

</xml_diff>